<commit_message>
Added strategy for testing
</commit_message>
<xml_diff>
--- a/Test_Results_HW02_Christopher_McKenzie.xlsx
+++ b/Test_Results_HW02_Christopher_McKenzie.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="85">
   <si>
     <t>Test ID</t>
   </si>
@@ -253,13 +253,31 @@
   </si>
   <si>
     <t>3NATB</t>
+  </si>
+  <si>
+    <t>Strategy:</t>
+  </si>
+  <si>
+    <t>including every possible triangle, incorrect input, and NotATriangle.</t>
+  </si>
+  <si>
+    <t>I determined I had enough tests when I could not think of any other unique way</t>
+  </si>
+  <si>
+    <t>to break the code. I believed that I could make more than 2 tests for each result,</t>
+  </si>
+  <si>
+    <t>but they would be redundant.</t>
+  </si>
+  <si>
+    <t>My strategy was to find at least 2 different inputs for each possible result,</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -269,6 +287,15 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -388,7 +415,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -402,6 +429,8 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -706,7 +735,7 @@
   <dimension ref="A1:J43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -922,6 +951,9 @@
       <c r="E8" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="G8" s="13" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A9" s="2" t="s">
@@ -939,6 +971,9 @@
       <c r="E9" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="G9" s="14" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
@@ -956,6 +991,9 @@
       <c r="E10" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="G10" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
@@ -973,6 +1011,9 @@
       <c r="E11" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="G11" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
@@ -990,6 +1031,9 @@
       <c r="E12" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="G12" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A13" s="2" t="s">
@@ -1006,6 +1050,9 @@
       </c>
       <c r="E13" s="3" t="s">
         <v>8</v>
+      </c>
+      <c r="G13" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
Moved written responses and tables to a word doc
</commit_message>
<xml_diff>
--- a/Test_Results_HW02_Christopher_McKenzie.xlsx
+++ b/Test_Results_HW02_Christopher_McKenzie.xlsx
@@ -350,7 +350,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -359,57 +359,38 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top style="medium">
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top/>
@@ -417,19 +398,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top/>
@@ -438,26 +410,38 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -761,8 +745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -775,249 +759,249 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
       <c r="G1" s="12"/>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="11" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="3" t="s">
+      <c r="D2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2" s="13">
         <v>14</v>
       </c>
-      <c r="I2" s="3">
+      <c r="I2" s="13">
         <v>14</v>
       </c>
-      <c r="J2" s="5">
+      <c r="J2" s="13">
         <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="3" t="s">
+      <c r="D3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H3" s="13">
         <v>14</v>
       </c>
-      <c r="I3" s="3">
+      <c r="I3" s="13">
         <v>14</v>
       </c>
-      <c r="J3" s="5">
+      <c r="J3" s="13">
         <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="3" t="s">
+      <c r="D4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H4" s="13">
         <v>3</v>
       </c>
-      <c r="I4" s="3">
+      <c r="I4" s="13">
         <v>11</v>
       </c>
-      <c r="J4" s="5">
+      <c r="J4" s="13">
         <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="3" t="s">
+      <c r="D5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="10" t="s">
+      <c r="G5" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5" s="13">
         <v>6</v>
       </c>
-      <c r="I5" s="3">
+      <c r="I5" s="13">
         <v>2</v>
       </c>
-      <c r="J5" s="5">
+      <c r="J5" s="13">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A6" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="3" t="s">
+      <c r="D6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>8</v>
       </c>
       <c r="G6" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="H6" s="1">
+      <c r="H6" s="13">
         <v>6</v>
       </c>
-      <c r="I6" s="1">
+      <c r="I6" s="13">
         <v>2</v>
       </c>
-      <c r="J6" s="6">
+      <c r="J6" s="13">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="3" t="s">
+      <c r="D7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="3" t="s">
+      <c r="D8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="2"/>
-      <c r="G8" s="13" t="s">
+      <c r="F8" s="1"/>
+      <c r="G8" s="2" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="3" t="s">
+      <c r="D9" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G9" s="14" t="s">
+      <c r="G9" s="3" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="2" t="s">
+      <c r="C10" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="6" t="s">
         <v>10</v>
       </c>
       <c r="G10" t="s">
@@ -1025,19 +1009,19 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" s="2" t="s">
+      <c r="C11" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="6" t="s">
         <v>10</v>
       </c>
       <c r="G11" t="s">
@@ -1045,19 +1029,19 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12" s="2" t="s">
+      <c r="C12" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="6" t="s">
         <v>10</v>
       </c>
       <c r="G12" t="s">
@@ -1065,19 +1049,19 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" s="2" t="s">
+      <c r="C13" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E13" s="5" t="s">
         <v>8</v>
       </c>
       <c r="G13" t="s">
@@ -1085,19 +1069,19 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="D14" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14" s="3" t="s">
+      <c r="D14" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="5" t="s">
         <v>8</v>
       </c>
       <c r="G14" t="s">
@@ -1105,19 +1089,19 @@
       </c>
     </row>
     <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E15" s="1" t="s">
+      <c r="D15" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="9" t="s">
         <v>8</v>
       </c>
       <c r="G15" t="s">
@@ -1125,19 +1109,19 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E16" s="5" t="s">
         <v>10</v>
       </c>
       <c r="G16" t="s">
@@ -1145,19 +1129,19 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E17" s="5" t="s">
         <v>8</v>
       </c>
       <c r="G17" t="s">
@@ -1165,19 +1149,19 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="E18" s="5" t="s">
         <v>10</v>
       </c>
       <c r="G18" t="s">
@@ -1185,19 +1169,19 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="E19" s="5" t="s">
         <v>10</v>
       </c>
       <c r="G19" t="s">
@@ -1205,19 +1189,19 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D20" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="E20" s="5" t="s">
         <v>8</v>
       </c>
       <c r="G20" t="s">
@@ -1225,56 +1209,56 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D21" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="E21" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D22" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="E22" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G22" s="13" t="s">
+      <c r="E22" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G22" s="2" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D23" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="E23" s="5" t="s">
         <v>10</v>
       </c>
       <c r="G23" t="s">
@@ -1282,342 +1266,342 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E24" s="3" t="s">
+      <c r="C24" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E25" s="3" t="s">
+      <c r="C25" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E25" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C26" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E26" s="3" t="s">
+      <c r="C26" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A27" s="2" t="s">
+      <c r="A27" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E27" s="3" t="s">
+      <c r="C27" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A28" s="2" t="s">
+      <c r="A28" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="D28" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="E28" s="3" t="s">
+      <c r="E28" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A29" s="4" t="s">
+      <c r="A29" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C29" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="D29" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="E29" s="9" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A30" s="3" t="s">
+      <c r="A30" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C30" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="D30" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E30" s="3" t="s">
+      <c r="E30" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A31" s="3" t="s">
+      <c r="A31" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C31" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="D31" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="E31" s="3" t="s">
+      <c r="E31" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A32" s="3" t="s">
+      <c r="A32" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C32" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="D32" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E32" s="3" t="s">
+      <c r="E32" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A33" s="2" t="s">
+      <c r="A33" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C33" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="D33" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E33" s="3" t="s">
+      <c r="E33" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A34" s="2" t="s">
+      <c r="A34" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B34" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C34" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="D34" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="E34" s="3" t="s">
+      <c r="E34" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A35" s="2" t="s">
+      <c r="A35" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B35" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C35" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="D35" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="E35" s="3" t="s">
+      <c r="E35" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A36" s="2" t="s">
+      <c r="A36" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B36" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="C36" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="D36" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="E36" s="3" t="s">
+      <c r="E36" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A37" s="2" t="s">
+      <c r="A37" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B37" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="C37" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="D37" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="E37" s="3" t="s">
+      <c r="E37" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A38" s="2" t="s">
+      <c r="A38" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B38" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C38" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E38" s="3" t="s">
+      <c r="C38" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E38" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A39" s="2" t="s">
+      <c r="A39" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B39" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C39" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E39" s="3" t="s">
+      <c r="C39" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E39" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A40" s="2" t="s">
+      <c r="A40" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B40" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C40" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E40" s="3" t="s">
+      <c r="C40" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E40" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A41" s="2" t="s">
+      <c r="A41" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="B41" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C41" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E41" s="3" t="s">
+      <c r="C41" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E41" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A42" s="2" t="s">
+      <c r="A42" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="B42" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="C42" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="D42" s="2" t="s">
+      <c r="D42" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="E42" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A43" s="4" t="s">
+      <c r="E42" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A43" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B43" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="C43" s="4" t="s">
+      <c r="C43" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="D43" s="4" t="s">
+      <c r="D43" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="E43" s="1" t="s">
+      <c r="E43" s="10" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>